<commit_message>
Patent paraları düzeltilmeden önce.
</commit_message>
<xml_diff>
--- a/Ofis Dosyalari/HAKEDISLER/2025/HAZIRAN 2025/2025 HAZIRAN AYI.xlsx
+++ b/Ofis Dosyalari/HAKEDISLER/2025/HAZIRAN 2025/2025 HAZIRAN AYI.xlsx
@@ -1042,9 +1042,9 @@
   <dimension ref="A1:N74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="K62" activeCellId="0" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2606,11 +2606,13 @@
       <c r="I43" s="26" t="n">
         <v>10000</v>
       </c>
-      <c r="J43" s="26"/>
+      <c r="J43" s="26" t="n">
+        <v>2500</v>
+      </c>
       <c r="K43" s="26"/>
       <c r="L43" s="27" t="n">
         <f aca="false">F43-G43-H43-I43-K43-J43</f>
-        <v>53200</v>
+        <v>50700</v>
       </c>
       <c r="M43" s="28"/>
     </row>
@@ -3283,10 +3285,12 @@
       <c r="J61" s="26" t="n">
         <v>10000</v>
       </c>
-      <c r="K61" s="26"/>
+      <c r="K61" s="26" t="n">
+        <v>61160</v>
+      </c>
       <c r="L61" s="27" t="n">
         <f aca="false">F61-G61-H61-I61-K61-J61</f>
-        <v>61160</v>
+        <v>0</v>
       </c>
       <c r="M61" s="28"/>
     </row>
@@ -3698,7 +3702,7 @@
       </c>
       <c r="L74" s="48" t="n">
         <f aca="false">SUM(L3:L73)</f>
-        <v>3470430</v>
+        <v>3406770</v>
       </c>
     </row>
   </sheetData>

</xml_diff>